<commit_message>
Working on productController and saving data sent by post
</commit_message>
<xml_diff>
--- a/xcrud_db.xlsx
+++ b/xcrud_db.xlsx
@@ -6,23 +6,15 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Productos" r:id="rId3" sheetId="1"/>
+    <sheet name="Dashboard" r:id="rId3" sheetId="1"/>
+    <sheet name="Products" r:id="rId4" sheetId="2"/>
+    <sheet name="Users" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Hola mundo</t>
-  </si>
-  <si>
-    <t>Enger</t>
-  </si>
-  <si>
-    <t>Jimenez</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65,24 +57,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>